<commit_message>
yay. it looks better.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-BotswanaAMRSpecimen.xlsx
+++ b/output/StructureDefinition-BotswanaAMRSpecimen.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/BotswanaAMRSpecimen</t>
+    <t>http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/BotswanaAMRSpecimen</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-17T18:14:37-04:00</t>
+    <t>2025-06-25T00:42:48-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -439,7 +439,7 @@
     <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
   </si>
   <si>
-    <t>http://example.org/fhir/StructureDefinition/BotswanaAMR-Specimen</t>
+    <t>http://bw.health.gov/fhir/StructureDefinition/BotswanaAMR-Specimen</t>
   </si>
   <si>
     <t>Meta.profile</t>
@@ -698,7 +698,7 @@
     <t>The type can change the way that a specimen is handled and drives what kind of analyses can properly be performed on the specimen. It is frequently used in diagnostic work flow decision making systems.</t>
   </si>
   <si>
-    <t>http://example.org/fhir/ImplementationGuide/bw-amr-ig/ValueSet/botswana-amr-specimen-type-vs</t>
+    <t>http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/ValueSet/botswana-amr-specimen-type-vs</t>
   </si>
   <si>
     <t>.code</t>
@@ -1567,7 +1567,7 @@
     <col min="23" max="23" width="16.40625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="15.85546875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="50.578125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="83.078125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="84.33203125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.2734375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.1171875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.56640625" customWidth="true" bestFit="true"/>

</xml_diff>